<commit_message>
Update -able to change P
</commit_message>
<xml_diff>
--- a/forecast_comparison_summary.xlsx
+++ b/forecast_comparison_summary.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,30 +455,20 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>P10</t>
+          <t>Amazon Mean Forecast</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>P90</t>
+          <t>Amazon P70 Forecast</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Amazon Mean Forecast</t>
+          <t>Amazon P80 Forecast</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Amazon P70 Forecast</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Amazon P80 Forecast</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Amazon P90 Forecast</t>
         </is>
@@ -494,24 +484,18 @@
         <v>45613</v>
       </c>
       <c r="C2" t="n">
-        <v>233</v>
+        <v>308</v>
       </c>
       <c r="D2" t="n">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="E2" t="n">
-        <v>344</v>
+        <v>168</v>
       </c>
       <c r="F2" t="n">
-        <v>142</v>
+        <v>192</v>
       </c>
       <c r="G2" t="n">
-        <v>168</v>
-      </c>
-      <c r="H2" t="n">
-        <v>192</v>
-      </c>
-      <c r="I2" t="n">
         <v>228</v>
       </c>
     </row>
@@ -525,24 +509,18 @@
         <v>45620</v>
       </c>
       <c r="C3" t="n">
-        <v>328</v>
+        <v>406</v>
       </c>
       <c r="D3" t="n">
-        <v>206</v>
+        <v>316</v>
       </c>
       <c r="E3" t="n">
-        <v>437</v>
+        <v>385</v>
       </c>
       <c r="F3" t="n">
-        <v>316</v>
+        <v>497</v>
       </c>
       <c r="G3" t="n">
-        <v>385</v>
-      </c>
-      <c r="H3" t="n">
-        <v>497</v>
-      </c>
-      <c r="I3" t="n">
         <v>685</v>
       </c>
     </row>
@@ -556,24 +534,18 @@
         <v>45627</v>
       </c>
       <c r="C4" t="n">
-        <v>317</v>
+        <v>393</v>
       </c>
       <c r="D4" t="n">
-        <v>213</v>
+        <v>316</v>
       </c>
       <c r="E4" t="n">
-        <v>427</v>
+        <v>385</v>
       </c>
       <c r="F4" t="n">
-        <v>316</v>
+        <v>497</v>
       </c>
       <c r="G4" t="n">
-        <v>385</v>
-      </c>
-      <c r="H4" t="n">
-        <v>497</v>
-      </c>
-      <c r="I4" t="n">
         <v>685</v>
       </c>
     </row>
@@ -587,24 +559,18 @@
         <v>45634</v>
       </c>
       <c r="C5" t="n">
-        <v>223</v>
+        <v>299</v>
       </c>
       <c r="D5" t="n">
-        <v>110</v>
+        <v>352</v>
       </c>
       <c r="E5" t="n">
-        <v>327</v>
+        <v>430</v>
       </c>
       <c r="F5" t="n">
-        <v>352</v>
+        <v>536</v>
       </c>
       <c r="G5" t="n">
-        <v>430</v>
-      </c>
-      <c r="H5" t="n">
-        <v>536</v>
-      </c>
-      <c r="I5" t="n">
         <v>709</v>
       </c>
     </row>
@@ -618,24 +584,18 @@
         <v>45641</v>
       </c>
       <c r="C6" t="n">
-        <v>125</v>
+        <v>207</v>
       </c>
       <c r="D6" t="n">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="E6" t="n">
-        <v>242</v>
+        <v>197</v>
       </c>
       <c r="F6" t="n">
-        <v>164</v>
+        <v>234</v>
       </c>
       <c r="G6" t="n">
-        <v>197</v>
-      </c>
-      <c r="H6" t="n">
-        <v>234</v>
-      </c>
-      <c r="I6" t="n">
         <v>291</v>
       </c>
     </row>
@@ -649,24 +609,18 @@
         <v>45648</v>
       </c>
       <c r="C7" t="n">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="D7" t="n">
-        <v>-22</v>
+        <v>167</v>
       </c>
       <c r="E7" t="n">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F7" t="n">
-        <v>167</v>
+        <v>241</v>
       </c>
       <c r="G7" t="n">
-        <v>202</v>
-      </c>
-      <c r="H7" t="n">
-        <v>241</v>
-      </c>
-      <c r="I7" t="n">
         <v>303</v>
       </c>
     </row>
@@ -680,24 +634,18 @@
         <v>45655</v>
       </c>
       <c r="C8" t="n">
-        <v>93</v>
+        <v>169</v>
       </c>
       <c r="D8" t="n">
-        <v>-29</v>
+        <v>124</v>
       </c>
       <c r="E8" t="n">
-        <v>212</v>
+        <v>150</v>
       </c>
       <c r="F8" t="n">
-        <v>124</v>
+        <v>181</v>
       </c>
       <c r="G8" t="n">
-        <v>150</v>
-      </c>
-      <c r="H8" t="n">
-        <v>181</v>
-      </c>
-      <c r="I8" t="n">
         <v>229</v>
       </c>
     </row>
@@ -711,24 +659,18 @@
         <v>45662</v>
       </c>
       <c r="C9" t="n">
-        <v>105</v>
+        <v>184</v>
       </c>
       <c r="D9" t="n">
-        <v>-13</v>
+        <v>124</v>
       </c>
       <c r="E9" t="n">
-        <v>214</v>
+        <v>150</v>
       </c>
       <c r="F9" t="n">
-        <v>124</v>
+        <v>180</v>
       </c>
       <c r="G9" t="n">
-        <v>150</v>
-      </c>
-      <c r="H9" t="n">
-        <v>180</v>
-      </c>
-      <c r="I9" t="n">
         <v>228</v>
       </c>
     </row>
@@ -742,24 +684,18 @@
         <v>45669</v>
       </c>
       <c r="C10" t="n">
-        <v>96</v>
+        <v>172</v>
       </c>
       <c r="D10" t="n">
-        <v>-19</v>
+        <v>122</v>
       </c>
       <c r="E10" t="n">
-        <v>208</v>
+        <v>148</v>
       </c>
       <c r="F10" t="n">
-        <v>122</v>
+        <v>176</v>
       </c>
       <c r="G10" t="n">
-        <v>148</v>
-      </c>
-      <c r="H10" t="n">
-        <v>176</v>
-      </c>
-      <c r="I10" t="n">
         <v>220</v>
       </c>
     </row>
@@ -773,24 +709,18 @@
         <v>45676</v>
       </c>
       <c r="C11" t="n">
-        <v>82</v>
+        <v>160</v>
       </c>
       <c r="D11" t="n">
-        <v>-29</v>
+        <v>124</v>
       </c>
       <c r="E11" t="n">
-        <v>194</v>
+        <v>151</v>
       </c>
       <c r="F11" t="n">
-        <v>124</v>
+        <v>180</v>
       </c>
       <c r="G11" t="n">
-        <v>151</v>
-      </c>
-      <c r="H11" t="n">
-        <v>180</v>
-      </c>
-      <c r="I11" t="n">
         <v>227</v>
       </c>
     </row>
@@ -804,24 +734,18 @@
         <v>45683</v>
       </c>
       <c r="C12" t="n">
-        <v>82</v>
+        <v>161</v>
       </c>
       <c r="D12" t="n">
-        <v>-27</v>
+        <v>128</v>
       </c>
       <c r="E12" t="n">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="F12" t="n">
-        <v>128</v>
+        <v>188</v>
       </c>
       <c r="G12" t="n">
-        <v>156</v>
-      </c>
-      <c r="H12" t="n">
-        <v>188</v>
-      </c>
-      <c r="I12" t="n">
         <v>238</v>
       </c>
     </row>
@@ -835,24 +759,18 @@
         <v>45690</v>
       </c>
       <c r="C13" t="n">
-        <v>96</v>
+        <v>174</v>
       </c>
       <c r="D13" t="n">
-        <v>-12</v>
+        <v>132</v>
       </c>
       <c r="E13" t="n">
-        <v>199</v>
+        <v>161</v>
       </c>
       <c r="F13" t="n">
-        <v>132</v>
+        <v>194</v>
       </c>
       <c r="G13" t="n">
-        <v>161</v>
-      </c>
-      <c r="H13" t="n">
-        <v>194</v>
-      </c>
-      <c r="I13" t="n">
         <v>246</v>
       </c>
     </row>
@@ -866,24 +784,18 @@
         <v>45697</v>
       </c>
       <c r="C14" t="n">
-        <v>104</v>
+        <v>181</v>
       </c>
       <c r="D14" t="n">
-        <v>-6</v>
+        <v>128</v>
       </c>
       <c r="E14" t="n">
-        <v>214</v>
+        <v>156</v>
       </c>
       <c r="F14" t="n">
-        <v>128</v>
+        <v>187</v>
       </c>
       <c r="G14" t="n">
-        <v>156</v>
-      </c>
-      <c r="H14" t="n">
-        <v>187</v>
-      </c>
-      <c r="I14" t="n">
         <v>237</v>
       </c>
     </row>
@@ -897,24 +809,18 @@
         <v>45704</v>
       </c>
       <c r="C15" t="n">
-        <v>96</v>
+        <v>172</v>
       </c>
       <c r="D15" t="n">
-        <v>-16</v>
+        <v>126</v>
       </c>
       <c r="E15" t="n">
-        <v>209</v>
+        <v>153</v>
       </c>
       <c r="F15" t="n">
-        <v>126</v>
+        <v>185</v>
       </c>
       <c r="G15" t="n">
-        <v>153</v>
-      </c>
-      <c r="H15" t="n">
-        <v>185</v>
-      </c>
-      <c r="I15" t="n">
         <v>235</v>
       </c>
     </row>
@@ -928,24 +834,18 @@
         <v>45711</v>
       </c>
       <c r="C16" t="n">
-        <v>86</v>
+        <v>164</v>
       </c>
       <c r="D16" t="n">
-        <v>-35</v>
+        <v>129</v>
       </c>
       <c r="E16" t="n">
-        <v>197</v>
+        <v>157</v>
       </c>
       <c r="F16" t="n">
-        <v>129</v>
+        <v>191</v>
       </c>
       <c r="G16" t="n">
-        <v>157</v>
-      </c>
-      <c r="H16" t="n">
-        <v>191</v>
-      </c>
-      <c r="I16" t="n">
         <v>244</v>
       </c>
     </row>
@@ -959,24 +859,18 @@
         <v>45718</v>
       </c>
       <c r="C17" t="n">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="D17" t="n">
-        <v>-25</v>
+        <v>129</v>
       </c>
       <c r="E17" t="n">
-        <v>191</v>
+        <v>157</v>
       </c>
       <c r="F17" t="n">
-        <v>129</v>
+        <v>190</v>
       </c>
       <c r="G17" t="n">
-        <v>157</v>
-      </c>
-      <c r="H17" t="n">
-        <v>190</v>
-      </c>
-      <c r="I17" t="n">
         <v>243</v>
       </c>
     </row>
@@ -990,24 +884,18 @@
         <v>45725</v>
       </c>
       <c r="C18" t="n">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="D18" t="n">
-        <v>-17</v>
+        <v>126</v>
       </c>
       <c r="E18" t="n">
-        <v>206</v>
+        <v>153</v>
       </c>
       <c r="F18" t="n">
-        <v>126</v>
+        <v>185</v>
       </c>
       <c r="G18" t="n">
-        <v>153</v>
-      </c>
-      <c r="H18" t="n">
-        <v>185</v>
-      </c>
-      <c r="I18" t="n">
         <v>235</v>
       </c>
     </row>
@@ -1021,24 +909,18 @@
         <v>45732</v>
       </c>
       <c r="C19" t="n">
-        <v>94</v>
+        <v>176</v>
       </c>
       <c r="D19" t="n">
-        <v>-14</v>
+        <v>124</v>
       </c>
       <c r="E19" t="n">
-        <v>205</v>
+        <v>150</v>
       </c>
       <c r="F19" t="n">
-        <v>124</v>
+        <v>180</v>
       </c>
       <c r="G19" t="n">
-        <v>150</v>
-      </c>
-      <c r="H19" t="n">
-        <v>180</v>
-      </c>
-      <c r="I19" t="n">
         <v>228</v>
       </c>
     </row>
@@ -1052,24 +934,18 @@
         <v>45739</v>
       </c>
       <c r="C20" t="n">
-        <v>77</v>
+        <v>156</v>
       </c>
       <c r="D20" t="n">
-        <v>-28</v>
+        <v>138</v>
       </c>
       <c r="E20" t="n">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="F20" t="n">
-        <v>138</v>
+        <v>202</v>
       </c>
       <c r="G20" t="n">
-        <v>167</v>
-      </c>
-      <c r="H20" t="n">
-        <v>202</v>
-      </c>
-      <c r="I20" t="n">
         <v>257</v>
       </c>
     </row>
@@ -1083,24 +959,18 @@
         <v>45746</v>
       </c>
       <c r="C21" t="n">
-        <v>59</v>
+        <v>137</v>
       </c>
       <c r="D21" t="n">
-        <v>-49</v>
+        <v>123</v>
       </c>
       <c r="E21" t="n">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="F21" t="n">
-        <v>123</v>
+        <v>183</v>
       </c>
       <c r="G21" t="n">
-        <v>150</v>
-      </c>
-      <c r="H21" t="n">
-        <v>183</v>
-      </c>
-      <c r="I21" t="n">
         <v>235</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Shows best percentile but under perform
</commit_message>
<xml_diff>
--- a/forecast_comparison_summary.xlsx
+++ b/forecast_comparison_summary.xlsx
@@ -484,7 +484,7 @@
         <v>45613</v>
       </c>
       <c r="C2" t="n">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D2" t="n">
         <v>142</v>
@@ -509,7 +509,7 @@
         <v>45620</v>
       </c>
       <c r="C3" t="n">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="D3" t="n">
         <v>316</v>
@@ -534,7 +534,7 @@
         <v>45627</v>
       </c>
       <c r="C4" t="n">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D4" t="n">
         <v>316</v>
@@ -559,7 +559,7 @@
         <v>45634</v>
       </c>
       <c r="C5" t="n">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D5" t="n">
         <v>352</v>
@@ -584,7 +584,7 @@
         <v>45641</v>
       </c>
       <c r="C6" t="n">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="D6" t="n">
         <v>164</v>
@@ -609,7 +609,7 @@
         <v>45648</v>
       </c>
       <c r="C7" t="n">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D7" t="n">
         <v>167</v>
@@ -634,7 +634,7 @@
         <v>45655</v>
       </c>
       <c r="C8" t="n">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="D8" t="n">
         <v>124</v>
@@ -659,7 +659,7 @@
         <v>45662</v>
       </c>
       <c r="C9" t="n">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D9" t="n">
         <v>124</v>
@@ -684,7 +684,7 @@
         <v>45669</v>
       </c>
       <c r="C10" t="n">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D10" t="n">
         <v>122</v>
@@ -709,7 +709,7 @@
         <v>45676</v>
       </c>
       <c r="C11" t="n">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D11" t="n">
         <v>124</v>
@@ -734,7 +734,7 @@
         <v>45683</v>
       </c>
       <c r="C12" t="n">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D12" t="n">
         <v>128</v>
@@ -759,7 +759,7 @@
         <v>45690</v>
       </c>
       <c r="C13" t="n">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D13" t="n">
         <v>132</v>
@@ -784,7 +784,7 @@
         <v>45697</v>
       </c>
       <c r="C14" t="n">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D14" t="n">
         <v>128</v>
@@ -809,7 +809,7 @@
         <v>45704</v>
       </c>
       <c r="C15" t="n">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D15" t="n">
         <v>126</v>
@@ -834,7 +834,7 @@
         <v>45711</v>
       </c>
       <c r="C16" t="n">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D16" t="n">
         <v>129</v>
@@ -859,7 +859,7 @@
         <v>45718</v>
       </c>
       <c r="C17" t="n">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D17" t="n">
         <v>129</v>
@@ -884,7 +884,7 @@
         <v>45725</v>
       </c>
       <c r="C18" t="n">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D18" t="n">
         <v>126</v>
@@ -909,7 +909,7 @@
         <v>45732</v>
       </c>
       <c r="C19" t="n">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D19" t="n">
         <v>124</v>
@@ -934,7 +934,7 @@
         <v>45739</v>
       </c>
       <c r="C20" t="n">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D20" t="n">
         <v>138</v>
@@ -959,7 +959,7 @@
         <v>45746</v>
       </c>
       <c r="C21" t="n">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="D21" t="n">
         <v>123</v>

</xml_diff>

<commit_message>
Working Version with One ASIN
</commit_message>
<xml_diff>
--- a/forecast_comparison_summary.xlsx
+++ b/forecast_comparison_summary.xlsx
@@ -462,19 +462,19 @@
         <v>45620</v>
       </c>
       <c r="B2" t="n">
-        <v>136.9818513185937</v>
+        <v>468.1561649076668</v>
       </c>
       <c r="C2" t="n">
-        <v>146</v>
+        <v>701</v>
       </c>
       <c r="D2" t="n">
-        <v>174</v>
+        <v>857</v>
       </c>
       <c r="E2" t="n">
-        <v>201</v>
+        <v>1079</v>
       </c>
       <c r="F2" t="n">
-        <v>242</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="3">
@@ -482,19 +482,19 @@
         <v>45627</v>
       </c>
       <c r="B3" t="n">
-        <v>168.4416160175068</v>
+        <v>532.1156751534114</v>
       </c>
       <c r="C3" t="n">
-        <v>98</v>
+        <v>266</v>
       </c>
       <c r="D3" t="n">
-        <v>115</v>
+        <v>321</v>
       </c>
       <c r="E3" t="n">
-        <v>131</v>
+        <v>383</v>
       </c>
       <c r="F3" t="n">
-        <v>155</v>
+        <v>480</v>
       </c>
     </row>
     <row r="4">
@@ -502,19 +502,19 @@
         <v>45634</v>
       </c>
       <c r="B4" t="n">
-        <v>169.914628026526</v>
+        <v>457.7327641261022</v>
       </c>
       <c r="C4" t="n">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="D4" t="n">
-        <v>107</v>
+        <v>167</v>
       </c>
       <c r="E4" t="n">
-        <v>123</v>
+        <v>196</v>
       </c>
       <c r="F4" t="n">
-        <v>147</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5">
@@ -522,19 +522,19 @@
         <v>45641</v>
       </c>
       <c r="B5" t="n">
-        <v>142.2947777098215</v>
+        <v>317.5540424429</v>
       </c>
       <c r="C5" t="n">
-        <v>107</v>
+        <v>173</v>
       </c>
       <c r="D5" t="n">
-        <v>129</v>
+        <v>208</v>
       </c>
       <c r="E5" t="n">
-        <v>151</v>
+        <v>247</v>
       </c>
       <c r="F5" t="n">
-        <v>186</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6">
@@ -542,19 +542,19 @@
         <v>45648</v>
       </c>
       <c r="B6" t="n">
-        <v>109.4664126188083</v>
+        <v>215.533517665481</v>
       </c>
       <c r="C6" t="n">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="D6" t="n">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="E6" t="n">
-        <v>120</v>
+        <v>175</v>
       </c>
       <c r="F6" t="n">
-        <v>146</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7">
@@ -562,19 +562,19 @@
         <v>45655</v>
       </c>
       <c r="B7" t="n">
-        <v>96.11049351104116</v>
+        <v>195.3814903846867</v>
       </c>
       <c r="C7" t="n">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="D7" t="n">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="E7" t="n">
-        <v>113</v>
+        <v>156</v>
       </c>
       <c r="F7" t="n">
-        <v>138</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8">
@@ -582,19 +582,19 @@
         <v>45662</v>
       </c>
       <c r="B8" t="n">
-        <v>105.7529104100227</v>
+        <v>221.8929296655804</v>
       </c>
       <c r="C8" t="n">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="D8" t="n">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="E8" t="n">
-        <v>115</v>
+        <v>165</v>
       </c>
       <c r="F8" t="n">
-        <v>141</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9">
@@ -602,19 +602,19 @@
         <v>45669</v>
       </c>
       <c r="B9" t="n">
-        <v>121.0872696606129</v>
+        <v>240.1185641152562</v>
       </c>
       <c r="C9" t="n">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="D9" t="n">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="E9" t="n">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="F9" t="n">
-        <v>136</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10">
@@ -622,19 +622,19 @@
         <v>45676</v>
       </c>
       <c r="B10" t="n">
-        <v>123.8774592370909</v>
+        <v>235.6136802083513</v>
       </c>
       <c r="C10" t="n">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="D10" t="n">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="E10" t="n">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="F10" t="n">
-        <v>134</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11">
@@ -642,19 +642,19 @@
         <v>45683</v>
       </c>
       <c r="B11" t="n">
-        <v>111.9007166143139</v>
+        <v>232.2287374602311</v>
       </c>
       <c r="C11" t="n">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="D11" t="n">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="E11" t="n">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="F11" t="n">
-        <v>146</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12">
@@ -662,19 +662,19 @@
         <v>45690</v>
       </c>
       <c r="B12" t="n">
-        <v>96.95746653853925</v>
+        <v>245.9224817702768</v>
       </c>
       <c r="C12" t="n">
-        <v>89</v>
+        <v>142</v>
       </c>
       <c r="D12" t="n">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="E12" t="n">
-        <v>126</v>
+        <v>207</v>
       </c>
       <c r="F12" t="n">
-        <v>156</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13">
@@ -682,19 +682,19 @@
         <v>45697</v>
       </c>
       <c r="B13" t="n">
-        <v>90.46160616357912</v>
+        <v>260.7051362051131</v>
       </c>
       <c r="C13" t="n">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="D13" t="n">
-        <v>106</v>
+        <v>165</v>
       </c>
       <c r="E13" t="n">
-        <v>125</v>
+        <v>199</v>
       </c>
       <c r="F13" t="n">
-        <v>155</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14">
@@ -702,19 +702,19 @@
         <v>45704</v>
       </c>
       <c r="B14" t="n">
-        <v>94.18715344996073</v>
+        <v>253.9997037880444</v>
       </c>
       <c r="C14" t="n">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="D14" t="n">
-        <v>99</v>
+        <v>166</v>
       </c>
       <c r="E14" t="n">
-        <v>117</v>
+        <v>198</v>
       </c>
       <c r="F14" t="n">
-        <v>144</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15">
@@ -722,19 +722,19 @@
         <v>45711</v>
       </c>
       <c r="B15" t="n">
-        <v>103.1471170533232</v>
+        <v>230.8431160633121</v>
       </c>
       <c r="C15" t="n">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="D15" t="n">
-        <v>97</v>
+        <v>158</v>
       </c>
       <c r="E15" t="n">
-        <v>115</v>
+        <v>189</v>
       </c>
       <c r="F15" t="n">
-        <v>144</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16">
@@ -742,19 +742,19 @@
         <v>45718</v>
       </c>
       <c r="B16" t="n">
-        <v>112.139807459956</v>
+        <v>217.6013250812106</v>
       </c>
       <c r="C16" t="n">
-        <v>82</v>
+        <v>131</v>
       </c>
       <c r="D16" t="n">
-        <v>99</v>
+        <v>160</v>
       </c>
       <c r="E16" t="n">
-        <v>118</v>
+        <v>193</v>
       </c>
       <c r="F16" t="n">
-        <v>148</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17">
@@ -762,19 +762,19 @@
         <v>45725</v>
       </c>
       <c r="B17" t="n">
-        <v>116.8763710020518</v>
+        <v>223.3925503230307</v>
       </c>
       <c r="C17" t="n">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="D17" t="n">
-        <v>98</v>
+        <v>163</v>
       </c>
       <c r="E17" t="n">
-        <v>117</v>
+        <v>196</v>
       </c>
       <c r="F17" t="n">
-        <v>146</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18">
@@ -782,19 +782,19 @@
         <v>45732</v>
       </c>
       <c r="B18" t="n">
-        <v>112.2331903575082</v>
+        <v>222.8242736541926</v>
       </c>
       <c r="C18" t="n">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="D18" t="n">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="E18" t="n">
-        <v>109</v>
+        <v>180</v>
       </c>
       <c r="F18" t="n">
-        <v>137</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19">
@@ -802,19 +802,19 @@
         <v>45739</v>
       </c>
       <c r="B19" t="n">
-        <v>95.36470947862614</v>
+        <v>186.8141746494535</v>
       </c>
       <c r="C19" t="n">
-        <v>73</v>
+        <v>130</v>
       </c>
       <c r="D19" t="n">
-        <v>89</v>
+        <v>158</v>
       </c>
       <c r="E19" t="n">
-        <v>106</v>
+        <v>190</v>
       </c>
       <c r="F19" t="n">
-        <v>132</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20">
@@ -822,19 +822,19 @@
         <v>45746</v>
       </c>
       <c r="B20" t="n">
-        <v>72.3859039842106</v>
+        <v>124.3343996311871</v>
       </c>
       <c r="C20" t="n">
-        <v>81</v>
+        <v>140</v>
       </c>
       <c r="D20" t="n">
-        <v>98</v>
+        <v>170</v>
       </c>
       <c r="E20" t="n">
-        <v>116</v>
+        <v>207</v>
       </c>
       <c r="F20" t="n">
-        <v>144</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21">
@@ -842,19 +842,19 @@
         <v>45753</v>
       </c>
       <c r="B21" t="n">
-        <v>57.96628639897691</v>
+        <v>80.51744823513057</v>
       </c>
       <c r="C21" t="n">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="D21" t="n">
-        <v>88</v>
+        <v>151</v>
       </c>
       <c r="E21" t="n">
-        <v>106</v>
+        <v>181</v>
       </c>
       <c r="F21" t="n">
-        <v>134</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -908,7 +908,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -920,7 +920,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>375</t>
+          <t>666</t>
         </is>
       </c>
     </row>
@@ -932,7 +932,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>188</t>
         </is>
       </c>
     </row>
@@ -944,7 +944,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>170</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>100</t>
         </is>
       </c>
     </row>
@@ -968,7 +968,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>13493 units</t>
+          <t>18802 units</t>
         </is>
       </c>
     </row>
@@ -980,7 +980,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1900</t>
+          <t>4549</t>
         </is>
       </c>
     </row>
@@ -992,7 +992,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1050</t>
+          <t>2648</t>
         </is>
       </c>
     </row>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>618</t>
+          <t>1776</t>
         </is>
       </c>
     </row>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>532</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-12-08</t>
+          <t>2024-12-01</t>
         </is>
       </c>
     </row>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>81</t>
         </is>
       </c>
     </row>

</xml_diff>